<commit_message>
fix the table of investmentrelation
</commit_message>
<xml_diff>
--- a/数据字典问题/数据字典/总体数字字典.xlsx
+++ b/数据字典问题/数据字典/总体数字字典.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5730" uniqueCount="2065">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5746" uniqueCount="2073">
   <si>
     <t>公司代码</t>
   </si>
@@ -14546,6 +14546,30 @@
   </si>
   <si>
     <t>StyleOfGetStock</t>
+  </si>
+  <si>
+    <t>购买日</t>
+  </si>
+  <si>
+    <t>DateOfBuy</t>
+  </si>
+  <si>
+    <t>购买日的确定依据</t>
+  </si>
+  <si>
+    <t>DateOfBuyConfirmAccord</t>
+  </si>
+  <si>
+    <t>购买日至期末被购买方的收入</t>
+  </si>
+  <si>
+    <t>DateOfBuyToEndAcquireeIncome</t>
+  </si>
+  <si>
+    <t>购买日至期末被购买方的净利润</t>
+  </si>
+  <si>
+    <t>DateOfBuyToEndAcquireeProfit</t>
   </si>
 </sst>
 </file>
@@ -14555,7 +14579,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -14593,8 +14617,15 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Droid Sans Fallback"/>
-      <family val="2"/>
+      <name val="宋体"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -14643,7 +14674,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -14656,7 +14687,15 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -14668,7 +14707,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Normal" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -14681,7 +14720,7 @@
   <dimension ref="A1:E65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1186" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1199" activeCellId="0" sqref="E1199"/>
+      <selection pane="topLeft" activeCell="A1209" activeCellId="0" sqref="A1209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -34291,6 +34330,62 @@
       </c>
       <c r="E1204" s="0" t="s">
         <v>2053</v>
+      </c>
+    </row>
+    <row r="1205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1205" s="0" t="s">
+        <v>2065</v>
+      </c>
+      <c r="B1205" s="0" t="s">
+        <v>2066</v>
+      </c>
+      <c r="C1205" s="4" t="s">
+        <v>2051</v>
+      </c>
+      <c r="D1205" s="0" t="s">
+        <v>2052</v>
+      </c>
+    </row>
+    <row r="1206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1206" s="0" t="s">
+        <v>2067</v>
+      </c>
+      <c r="B1206" s="0" t="s">
+        <v>2068</v>
+      </c>
+      <c r="C1206" s="4" t="s">
+        <v>906</v>
+      </c>
+      <c r="D1206" s="0" t="s">
+        <v>2052</v>
+      </c>
+    </row>
+    <row r="1207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1207" s="5" t="s">
+        <v>2069</v>
+      </c>
+      <c r="B1207" s="0" t="s">
+        <v>2070</v>
+      </c>
+      <c r="C1207" s="4" t="s">
+        <v>2060</v>
+      </c>
+      <c r="D1207" s="0" t="s">
+        <v>2052</v>
+      </c>
+    </row>
+    <row r="1208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1208" s="5" t="s">
+        <v>2071</v>
+      </c>
+      <c r="B1208" s="4" t="s">
+        <v>2072</v>
+      </c>
+      <c r="C1208" s="4" t="s">
+        <v>2060</v>
+      </c>
+      <c r="D1208" s="0" t="s">
+        <v>2052</v>
       </c>
     </row>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
add the Djando and Echarts
</commit_message>
<xml_diff>
--- a/数据字典问题/数据字典/总体数字字典.xlsx
+++ b/数据字典问题/数据字典/总体数字字典.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="142" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="138" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5746" uniqueCount="2073">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5840" uniqueCount="2099">
   <si>
     <t>公司代码</t>
   </si>
@@ -14570,6 +14570,84 @@
   </si>
   <si>
     <t>DateOfBuyToEndAcquireeProfit</t>
+  </si>
+  <si>
+    <t>keyhotwords</t>
+  </si>
+  <si>
+    <t>关键热词</t>
+  </si>
+  <si>
+    <t>年份</t>
+  </si>
+  <si>
+    <t>newssentiment</t>
+  </si>
+  <si>
+    <t>公司情感分布</t>
+  </si>
+  <si>
+    <t>Vchar(45)</t>
+  </si>
+  <si>
+    <t>情感取向</t>
+  </si>
+  <si>
+    <t>sentiment</t>
+  </si>
+  <si>
+    <t>newsyearcountall</t>
+  </si>
+  <si>
+    <t>公司历时报道量</t>
+  </si>
+  <si>
+    <t>公司历年新闻数量</t>
+  </si>
+  <si>
+    <t>newscount</t>
+  </si>
+  <si>
+    <t>newssourcecount</t>
+  </si>
+  <si>
+    <t>公司新闻来源</t>
+  </si>
+  <si>
+    <t>十个主要新闻来源</t>
+  </si>
+  <si>
+    <t>tensource</t>
+  </si>
+  <si>
+    <t>newstimecount</t>
+  </si>
+  <si>
+    <t>公司新闻资讯发布时间</t>
+  </si>
+  <si>
+    <t>时间段</t>
+  </si>
+  <si>
+    <t>timesegment</t>
+  </si>
+  <si>
+    <t>报道数量</t>
+  </si>
+  <si>
+    <t>companyreportnumberchange</t>
+  </si>
+  <si>
+    <t>公司报道量变化</t>
+  </si>
+  <si>
+    <t>报道公司名称</t>
+  </si>
+  <si>
+    <t>reportcompany</t>
+  </si>
+  <si>
+    <t>reportnumber</t>
   </si>
 </sst>
 </file>
@@ -14579,7 +14657,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -14619,6 +14697,7 @@
       <color rgb="FF000000"/>
       <name val="宋体"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -14626,6 +14705,21 @@
       <color rgb="FF000000"/>
       <name val="Consolas"/>
       <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Droid Sans Fallback"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <family val="0"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -14674,7 +14768,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -14699,6 +14793,18 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -14707,7 +14813,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -14719,15 +14825,15 @@
   </sheetPr>
   <dimension ref="A1:E65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1186" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1209" activeCellId="0" sqref="A1209"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1210" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1226" activeCellId="0" sqref="E1226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.7124463519313"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.0042918454936"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.519313304721"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.8154506437768"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.8969957081545"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.7510729613734"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.519313304721"/>
@@ -34345,6 +34451,9 @@
       <c r="D1205" s="0" t="s">
         <v>2052</v>
       </c>
+      <c r="E1205" s="0" t="s">
+        <v>2053</v>
+      </c>
     </row>
     <row r="1206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1206" s="0" t="s">
@@ -34359,6 +34468,9 @@
       <c r="D1206" s="0" t="s">
         <v>2052</v>
       </c>
+      <c r="E1206" s="0" t="s">
+        <v>2053</v>
+      </c>
     </row>
     <row r="1207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1207" s="5" t="s">
@@ -34373,6 +34485,9 @@
       <c r="D1207" s="0" t="s">
         <v>2052</v>
       </c>
+      <c r="E1207" s="0" t="s">
+        <v>2053</v>
+      </c>
     </row>
     <row r="1208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1208" s="5" t="s">
@@ -34386,6 +34501,315 @@
       </c>
       <c r="D1208" s="0" t="s">
         <v>2052</v>
+      </c>
+      <c r="E1208" s="0" t="s">
+        <v>2053</v>
+      </c>
+    </row>
+    <row r="1209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1209" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1209" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1209" s="0" t="s">
+        <v>2051</v>
+      </c>
+      <c r="D1209" s="0" t="s">
+        <v>2073</v>
+      </c>
+      <c r="E1209" s="0" t="s">
+        <v>2074</v>
+      </c>
+    </row>
+    <row r="1210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1210" s="0" t="s">
+        <v>2075</v>
+      </c>
+      <c r="B1210" s="0" t="s">
+        <v>1533</v>
+      </c>
+      <c r="C1210" s="0" t="s">
+        <v>2051</v>
+      </c>
+      <c r="D1210" s="0" t="s">
+        <v>2073</v>
+      </c>
+      <c r="E1210" s="0" t="s">
+        <v>2074</v>
+      </c>
+    </row>
+    <row r="1211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1211" s="0" t="s">
+        <v>2074</v>
+      </c>
+      <c r="B1211" s="0" t="s">
+        <v>2073</v>
+      </c>
+      <c r="C1211" s="0" t="s">
+        <v>906</v>
+      </c>
+      <c r="D1211" s="0" t="s">
+        <v>2073</v>
+      </c>
+      <c r="E1211" s="0" t="s">
+        <v>2074</v>
+      </c>
+    </row>
+    <row r="1212" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1212" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1212" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1212" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1212" s="7" t="s">
+        <v>2076</v>
+      </c>
+      <c r="E1212" s="0" t="s">
+        <v>2077</v>
+      </c>
+    </row>
+    <row r="1213" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1213" s="6" t="s">
+        <v>2075</v>
+      </c>
+      <c r="B1213" s="7" t="s">
+        <v>1533</v>
+      </c>
+      <c r="C1213" s="8" t="s">
+        <v>2078</v>
+      </c>
+      <c r="D1213" s="7" t="s">
+        <v>2076</v>
+      </c>
+      <c r="E1213" s="0" t="s">
+        <v>2077</v>
+      </c>
+    </row>
+    <row r="1214" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1214" s="6" t="s">
+        <v>2079</v>
+      </c>
+      <c r="B1214" s="7" t="s">
+        <v>2080</v>
+      </c>
+      <c r="C1214" s="8" t="s">
+        <v>906</v>
+      </c>
+      <c r="D1214" s="7" t="s">
+        <v>2076</v>
+      </c>
+      <c r="E1214" s="0" t="s">
+        <v>2077</v>
+      </c>
+    </row>
+    <row r="1215" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1215" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1215" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1215" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1215" s="7" t="s">
+        <v>2081</v>
+      </c>
+      <c r="E1215" s="0" t="s">
+        <v>2082</v>
+      </c>
+    </row>
+    <row r="1216" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1216" s="6" t="s">
+        <v>2075</v>
+      </c>
+      <c r="B1216" s="7" t="s">
+        <v>1533</v>
+      </c>
+      <c r="C1216" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1216" s="7" t="s">
+        <v>2081</v>
+      </c>
+      <c r="E1216" s="0" t="s">
+        <v>2082</v>
+      </c>
+    </row>
+    <row r="1217" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1217" s="6" t="s">
+        <v>2083</v>
+      </c>
+      <c r="B1217" s="7" t="s">
+        <v>2084</v>
+      </c>
+      <c r="C1217" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1217" s="7" t="s">
+        <v>2081</v>
+      </c>
+      <c r="E1217" s="0" t="s">
+        <v>2082</v>
+      </c>
+    </row>
+    <row r="1218" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1218" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1218" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1218" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1218" s="7" t="s">
+        <v>2085</v>
+      </c>
+      <c r="E1218" s="0" t="s">
+        <v>2086</v>
+      </c>
+    </row>
+    <row r="1219" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1219" s="6" t="s">
+        <v>2087</v>
+      </c>
+      <c r="B1219" s="7" t="s">
+        <v>2088</v>
+      </c>
+      <c r="C1219" s="8" t="s">
+        <v>906</v>
+      </c>
+      <c r="D1219" s="7" t="s">
+        <v>2085</v>
+      </c>
+      <c r="E1219" s="0" t="s">
+        <v>2086</v>
+      </c>
+    </row>
+    <row r="1220" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1220" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1220" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1220" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1220" s="7" t="s">
+        <v>2089</v>
+      </c>
+      <c r="E1220" s="0" t="s">
+        <v>2090</v>
+      </c>
+    </row>
+    <row r="1221" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1221" s="6" t="s">
+        <v>2091</v>
+      </c>
+      <c r="B1221" s="7" t="s">
+        <v>2092</v>
+      </c>
+      <c r="C1221" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1221" s="7" t="s">
+        <v>2089</v>
+      </c>
+      <c r="E1221" s="0" t="s">
+        <v>2090</v>
+      </c>
+    </row>
+    <row r="1222" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1222" s="6" t="s">
+        <v>2093</v>
+      </c>
+      <c r="B1222" s="7" t="s">
+        <v>2084</v>
+      </c>
+      <c r="C1222" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1222" s="7" t="s">
+        <v>2089</v>
+      </c>
+      <c r="E1222" s="0" t="s">
+        <v>2090</v>
+      </c>
+    </row>
+    <row r="1223" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1223" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1223" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1223" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1223" s="7" t="s">
+        <v>2094</v>
+      </c>
+      <c r="E1223" s="0" t="s">
+        <v>2095</v>
+      </c>
+    </row>
+    <row r="1224" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1224" s="6" t="s">
+        <v>2096</v>
+      </c>
+      <c r="B1224" s="7" t="s">
+        <v>2097</v>
+      </c>
+      <c r="C1224" s="8" t="s">
+        <v>906</v>
+      </c>
+      <c r="D1224" s="7" t="s">
+        <v>2094</v>
+      </c>
+      <c r="E1224" s="0" t="s">
+        <v>2095</v>
+      </c>
+    </row>
+    <row r="1225" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1225" s="6" t="s">
+        <v>2075</v>
+      </c>
+      <c r="B1225" s="7" t="s">
+        <v>1533</v>
+      </c>
+      <c r="C1225" s="8" t="s">
+        <v>2078</v>
+      </c>
+      <c r="D1225" s="7" t="s">
+        <v>2094</v>
+      </c>
+      <c r="E1225" s="0" t="s">
+        <v>2095</v>
+      </c>
+    </row>
+    <row r="1226" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1226" s="6" t="s">
+        <v>2093</v>
+      </c>
+      <c r="B1226" s="7" t="s">
+        <v>2098</v>
+      </c>
+      <c r="C1226" s="8" t="s">
+        <v>2078</v>
+      </c>
+      <c r="D1226" s="7" t="s">
+        <v>2094</v>
+      </c>
+      <c r="E1226" s="0" t="s">
+        <v>2095</v>
       </c>
     </row>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>